<commit_message>
* IHM preliminaire pour banc de test
</commit_message>
<xml_diff>
--- a/code/Banc-de-test/TouchGFX/assets/texts/texts.xlsx
+++ b/code/Banc-de-test/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4167" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4971" uniqueCount="225">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -734,6 +734,106 @@
   </si>
   <si>
     <t xml:space="preserve">Choix du Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation de la voile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisez l'analyseur logique
+pour visualiser les communications
+entre le micro et les peripheriques
+I2C et SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation bateau: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Servo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--° (-- ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisez l'analyseur logique
+pour visualiser les communications
+entre le micro et les peripheriques
+I2C et SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisez l'analyseur logique
+pour visualiser les communications
+entre le micro et les peripheriques
+I2C et SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisez l'analyseur logique
+pour visualiser les communications
+entre le micro et les peripheriques
+I2C et SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C / SPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tension batterie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Complet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girouette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0V
+[0x000]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation
+plateau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0V
+[0x000]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotation
+plateau</t>
   </si>
 </sst>
 </file>
@@ -2343,7 +2443,7 @@
         <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10">
@@ -2360,7 +2460,7 @@
         <v>46</v>
       </c>
       <c r="F10" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11">
@@ -2377,7 +2477,7 @@
         <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>125</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12">
@@ -2394,7 +2494,7 @@
         <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>127</v>
+        <v>212</v>
       </c>
     </row>
     <row r="13">
@@ -2411,7 +2511,7 @@
         <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>129</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14">
@@ -2429,6 +2529,193 @@
       </c>
       <c r="F14" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>218</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>